<commit_message>
changes to align with previous working release
</commit_message>
<xml_diff>
--- a/Documents/web socket messages.xlsx
+++ b/Documents/web socket messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\david284\MMC-SERVER\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E41F2F-875C-4DF2-BD2F-7458F5C36149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7593A09C-AC57-4B0E-BE53-7C95F5762FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>TEACH_EVENT</t>
   </si>
@@ -39,9 +39,6 @@
     <t>UPDATE_EVENT_VARIABLE</t>
   </si>
   <si>
-    <t>REQUEST_EVENT_VARIABLE</t>
-  </si>
-  <si>
     <t>REQUEST_ALL_EVENT_VARIABLES</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>update_event_variable</t>
   </si>
   <si>
-    <t>REVAL (USES INDEX)</t>
-  </si>
-  <si>
     <t>requestEventVariablesByIndex</t>
   </si>
   <si>
@@ -97,6 +91,36 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Don't need to refresh all events as not using index</t>
+  </si>
+  <si>
+    <t>Only need to read the one variable</t>
+  </si>
+  <si>
+    <t>Not using this at the moment</t>
+  </si>
+  <si>
+    <t>using EVENT_TEACH_BY_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>REQUEST_EVENT_VARIABLE
+(REVAL - USES INDEX)</t>
+  </si>
+  <si>
+    <t>delete_all_events
+request_all_node_events</t>
+  </si>
+  <si>
+    <t>yes
+yes</t>
   </si>
 </sst>
 </file>
@@ -140,13 +164,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,156 +460,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E26"/>
+  <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="3.46484375" customWidth="1"/>
     <col min="2" max="2" width="36.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="30.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
+      <c r="F20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>8</v>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to event teaching - unused methods removed & unit tests updated
</commit_message>
<xml_diff>
--- a/Documents/web socket messages.xlsx
+++ b/Documents/web socket messages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\david284\MMC-SERVER\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7593A09C-AC57-4B0E-BE53-7C95F5762FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EDB0EA-4DEB-4396-93A5-C3437EE8F08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
-  <si>
-    <t>TEACH_EVENT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t xml:space="preserve">                    </t>
   </si>
@@ -36,9 +33,6 @@
     <t>EVENT_TEACH_BY_IDENTIFIER</t>
   </si>
   <si>
-    <t>UPDATE_EVENT_VARIABLE</t>
-  </si>
-  <si>
     <t>REQUEST_ALL_EVENT_VARIABLES</t>
   </si>
   <si>
@@ -57,18 +51,12 @@
     <t>event_teach_by_identifier</t>
   </si>
   <si>
-    <t>update_event_variable</t>
-  </si>
-  <si>
     <t>requestEventVariablesByIndex</t>
   </si>
   <si>
     <t>requestEventVariablesByIdentifier</t>
   </si>
   <si>
-    <t>teach_event</t>
-  </si>
-  <si>
     <t>MergAdminNode functions called</t>
   </si>
   <si>
@@ -78,12 +66,6 @@
     <t>requestEventVariableByIdentifier</t>
   </si>
   <si>
-    <t>UPDATE_EVENT_VARIABLE_BY_IDENTIFIER</t>
-  </si>
-  <si>
-    <t>updateEventVariableByIdentifier</t>
-  </si>
-  <si>
     <t>unit test?</t>
   </si>
   <si>
@@ -99,13 +81,7 @@
     <t>Don't need to refresh all events as not using index</t>
   </si>
   <si>
-    <t>Only need to read the one variable</t>
-  </si>
-  <si>
     <t>Not using this at the moment</t>
-  </si>
-  <si>
-    <t>using EVENT_TEACH_BY_IDENTIFIER</t>
   </si>
   <si>
     <t>--</t>
@@ -121,6 +97,12 @@
   <si>
     <t>yes
 yes</t>
+  </si>
+  <si>
+    <t>relies on index being updated</t>
+  </si>
+  <si>
+    <t>Request needs index, and will have changed if new event</t>
   </si>
 </sst>
 </file>
@@ -460,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G24"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -474,223 +456,142 @@
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="30.06640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B8" s="4"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>30</v>
+      <c r="F16" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>